<commit_message>
Sanity Testing-User Registration Flow is done
</commit_message>
<xml_diff>
--- a/out/production/NFHSLearn/com/NFHS/xls/Registration.xlsx
+++ b/out/production/NFHSLearn/com/NFHS/xls/Registration.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="51">
   <si>
     <t>TCID</t>
   </si>
@@ -246,10 +246,13 @@
     <t>User should  be registered successfully</t>
   </si>
   <si>
-    <t>bhabani.shankar115@weboapps.com</t>
-  </si>
-  <si>
     <t>test1234</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>bhabani.shankar200@weboapps.com</t>
   </si>
 </sst>
 </file>
@@ -926,6 +929,9 @@
       <c r="D10" s="20" t="s">
         <v>6</v>
       </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="C12" s="15"/>
@@ -1439,7 +1445,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1448,8 +1454,8 @@
     <col min="2" max="2" width="41.28515625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="28.5703125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="12" customFormat="1">
@@ -1477,16 +1483,16 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1">
       <c r="A2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="D2" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>

</xml_diff>